<commit_message>
Made final edits and ran tests.
</commit_message>
<xml_diff>
--- a/Tests/Test results.xlsx
+++ b/Tests/Test results.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Projects\Unity Tutorials - learn.unity.com\Create with Code\Junior Programmer - Object-Oriented Programming Submission\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFA8F86-32B0-467C-930D-3A8EDA098F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A9A121-1F18-4964-BAEB-67930D00554E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="17">
   <si>
     <t>Test No.</t>
   </si>
@@ -67,6 +76,15 @@
   </si>
   <si>
     <t>Losses</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Overall results</t>
+  </si>
+  <si>
+    <t>If the player selects the Truck or Light vehicle, it is possible to win more often than when all vehicles are controlled by the algorithm. However, this is not shown by the results when controlling the Heavy vehicle. If a future version is released, it may be useful to make the Heavy and Light vehicles easier to control.</t>
   </si>
 </sst>
 </file>
@@ -102,16 +120,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,9 +428,10 @@
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="29" width="3.77734375" customWidth="1"/>
     <col min="30" max="31" width="6.6640625" customWidth="1"/>
+    <col min="32" max="32" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +475,11 @@
         <v>10</v>
       </c>
       <c r="AE1" s="1"/>
+      <c r="AF1" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -540,12 +565,13 @@
       <c r="AE2" t="s">
         <v>13</v>
       </c>
+      <c r="AF2" s="4"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
@@ -563,47 +589,378 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3">
+        <f>COUNTIF($E3:$AC3, "W")</f>
+        <v>2</v>
+      </c>
+      <c r="AE3">
+        <f>COUNTIF($E3:$AC3, "L")</f>
+        <v>23</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD4">
+        <f>COUNTIF($E4:$AC4, "W")</f>
+        <v>21</v>
+      </c>
+      <c r="AE4">
+        <f>COUNTIF($E4:$AC4, "L")</f>
+        <v>4</v>
+      </c>
+      <c r="AF4" s="4"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" t="s">
+        <v>11</v>
+      </c>
+      <c r="U5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD5">
+        <f>COUNTIF($E5:$AC5, "W")</f>
+        <v>7</v>
+      </c>
+      <c r="AE5">
+        <f>COUNTIF($E5:$AC5, "L")</f>
+        <v>18</v>
+      </c>
+      <c r="AF5" s="4"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" t="s">
+        <v>14</v>
+      </c>
+      <c r="U6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6" t="s">
+        <v>11</v>
+      </c>
+      <c r="W6" t="s">
+        <v>11</v>
+      </c>
+      <c r="X6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD6">
+        <f>COUNTIF($E6:$AC6, "W")</f>
+        <v>2</v>
+      </c>
+      <c r="AE6">
+        <f>COUNTIF($E6:$AC6, "L")</f>
+        <v>23</v>
+      </c>
+      <c r="AF6" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AF3:AF6"/>
     <mergeCell ref="E1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>